<commit_message>
Updated club names and prediction features
</commit_message>
<xml_diff>
--- a/Soccer Machine/Club Names.xlsx
+++ b/Soccer Machine/Club Names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\Sports Stuff\The Machine\the-machine\Soccer Machine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FB6E84-3BBA-42FC-9F9B-D8CE5CC5EF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE272C8-D163-44D3-BC8B-756304BD235B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{66BF1EEF-F4F0-4B2A-B933-3562F007E550}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="351">
   <si>
     <t>Atlanta Utd</t>
   </si>
@@ -1060,6 +1060,36 @@
   </si>
   <si>
     <t>Charlotte FC</t>
+  </si>
+  <si>
+    <t>Malmo se</t>
+  </si>
+  <si>
+    <t>se Malmo</t>
+  </si>
+  <si>
+    <t>Fenerbahce tr</t>
+  </si>
+  <si>
+    <t>Ferencvaros hu</t>
+  </si>
+  <si>
+    <t>dk Brondby</t>
+  </si>
+  <si>
+    <t>Brondby IF</t>
+  </si>
+  <si>
+    <t>Brondby dk</t>
+  </si>
+  <si>
+    <t>hu Ferencvaros</t>
+  </si>
+  <si>
+    <t>Ferencvarosi TC</t>
+  </si>
+  <si>
+    <t>tr Fenerbahce</t>
   </si>
 </sst>
 </file>
@@ -1414,10 +1444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C69D7B6-E6BC-4B78-B3F8-3995E9E68E3A}">
-  <dimension ref="A1:E257"/>
+  <dimension ref="A1:E265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="B265" sqref="B265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3013,1247 +3043,1335 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>57</v>
+        <v>218</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>202</v>
+        <v>341</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>57</v>
+        <v>218</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>170</v>
+        <v>58</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>170</v>
+        <v>58</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>113</v>
+        <v>177</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>113</v>
+        <v>177</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="B152" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C151" s="1" t="s">
+      <c r="C152" s="1" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>87</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
+        <v>87</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>89</v>
       </c>
-      <c r="B153" s="1" t="s">
+      <c r="B154" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="C154" s="1" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B156" s="1" t="s">
+      <c r="B157" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="C157" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>91</v>
       </c>
-      <c r="B157" s="1" t="s">
+      <c r="B158" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C157" s="1" t="s">
+      <c r="C158" s="1" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>180</v>
+        <v>116</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>180</v>
+        <v>116</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>306</v>
+        <v>217</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E163" s="1"/>
+        <v>176</v>
+      </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>101</v>
+        <v>180</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>101</v>
+        <v>180</v>
       </c>
       <c r="E164" s="1"/>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>119</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E165" s="1"/>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B172" s="1" t="s">
+      <c r="B173" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="C172" s="1" t="s">
+      <c r="C173" s="1" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>94</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C173" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>89</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>91</v>
       </c>
-      <c r="B176" s="1" t="s">
+      <c r="B177" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="C176" s="1" t="s">
+      <c r="C177" s="1" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E185" s="1"/>
+        <v>173</v>
+      </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>177</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="E186" s="1"/>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>218</v>
+        <v>181</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>175</v>
+        <v>218</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>175</v>
+        <v>218</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>175</v>
+        <v>218</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>239</v>
+        <v>182</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>240</v>
+        <v>336</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>239</v>
+        <v>182</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>95</v>
+      <c r="A195" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>241</v>
+        <v>337</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>95</v>
+        <v>179</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" s="1" t="s">
-        <v>272</v>
+      <c r="A197" t="s">
+        <v>95</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>231</v>
+        <v>95</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>121</v>
+        <v>272</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>246</v>
+        <v>347</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>121</v>
+        <v>346</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>273</v>
+        <v>233</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>235</v>
+        <v>121</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>235</v>
+        <v>121</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>159</v>
+        <v>221</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>251</v>
+        <v>343</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>159</v>
+        <v>221</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>237</v>
+        <v>273</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>55</v>
+        <v>273</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>253</v>
+        <v>344</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>55</v>
+        <v>234</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>118</v>
+        <v>235</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>118</v>
+        <v>235</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>223</v>
+        <v>159</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>223</v>
+        <v>159</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>135</v>
+        <v>237</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>135</v>
+        <v>237</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>136</v>
+        <v>55</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>136</v>
+        <v>55</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>220</v>
+        <v>118</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>220</v>
+        <v>118</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>161</v>
+        <v>223</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>161</v>
+        <v>223</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>238</v>
+        <v>135</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>238</v>
+        <v>135</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>224</v>
+        <v>136</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>224</v>
+        <v>136</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>226</v>
+        <v>138</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>226</v>
+        <v>138</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>88</v>
+      <c r="A220" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>88</v>
+        <v>161</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A225" s="1" t="s">
-        <v>64</v>
+      <c r="A225" t="s">
+        <v>88</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>223</v>
+        <v>64</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>223</v>
+        <v>64</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>121</v>
+        <v>229</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>121</v>
+        <v>229</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>118</v>
+        <v>239</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>118</v>
+        <v>239</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>272</v>
+        <v>236</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>55</v>
+        <v>227</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>55</v>
+        <v>227</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>95</v>
+      <c r="A238" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
-        <v>88</v>
+      <c r="A239" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>88</v>
+        <v>231</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
-        <v>135</v>
+        <v>272</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>288</v>
+        <v>345</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>135</v>
+        <v>346</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>136</v>
+        <v>220</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>136</v>
+        <v>220</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>138</v>
+        <v>55</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>138</v>
+        <v>55</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>238</v>
+        <v>64</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>238</v>
+        <v>64</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244" s="1" t="s">
-        <v>233</v>
+      <c r="A244" t="s">
+        <v>95</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>233</v>
+        <v>95</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A245" s="1" t="s">
-        <v>273</v>
+      <c r="A245" t="s">
+        <v>88</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>234</v>
+        <v>88</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>224</v>
+        <v>138</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>224</v>
+        <v>138</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>232</v>
+        <v>273</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
-        <v>222</v>
+        <v>273</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>300</v>
+        <v>348</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>222</v>
+        <v>349</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>228</v>
+        <v>159</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>228</v>
+        <v>159</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>219</v>
+        <v>161</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>219</v>
+        <v>161</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B257" s="1" t="s">
+      <c r="B265" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C257" s="1" t="s">
+      <c r="C265" s="1" t="s">
         <v>235</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Bovada links for Big 5
</commit_message>
<xml_diff>
--- a/Soccer Machine/Club Names.xlsx
+++ b/Soccer Machine/Club Names.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\Sports Stuff\The Machine\the-machine\Soccer Machine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\SportsStuff\TheMachine\the-machine\Soccer Machine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36871F2-F9F7-4FCE-8C50-ACE03FF57E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BCA985-0AA4-49A9-96A7-EF454C6E1CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{66BF1EEF-F4F0-4B2A-B933-3562F007E550}"/>
+    <workbookView xWindow="-23148" yWindow="3804" windowWidth="23256" windowHeight="12576" xr2:uid="{66BF1EEF-F4F0-4B2A-B933-3562F007E550}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="370">
   <si>
     <t>Atlanta Utd</t>
   </si>
@@ -1090,6 +1090,63 @@
   </si>
   <si>
     <t>tr Fenerbahce</t>
+  </si>
+  <si>
+    <t>Nottingham Forest</t>
+  </si>
+  <si>
+    <t>Nott'ham Forest</t>
+  </si>
+  <si>
+    <t>Bournemouth</t>
+  </si>
+  <si>
+    <t>Fulham</t>
+  </si>
+  <si>
+    <t>Real Valladolid</t>
+  </si>
+  <si>
+    <t>Valladolid</t>
+  </si>
+  <si>
+    <t>Almería</t>
+  </si>
+  <si>
+    <t>Almeria</t>
+  </si>
+  <si>
+    <t>Girona</t>
+  </si>
+  <si>
+    <t>Schalke 04</t>
+  </si>
+  <si>
+    <t>Werder Bremen</t>
+  </si>
+  <si>
+    <t>Toulouse</t>
+  </si>
+  <si>
+    <t>AC Ajaccio</t>
+  </si>
+  <si>
+    <t>Ajaccio</t>
+  </si>
+  <si>
+    <t>Auxerre</t>
+  </si>
+  <si>
+    <t>AJ Auxerre</t>
+  </si>
+  <si>
+    <t>Lecce</t>
+  </si>
+  <si>
+    <t>Cremonese</t>
+  </si>
+  <si>
+    <t>Monza</t>
   </si>
 </sst>
 </file>
@@ -1444,10 +1501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C69D7B6-E6BC-4B78-B3F8-3995E9E68E3A}">
-  <dimension ref="A1:E265"/>
+  <dimension ref="A1:E279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="B265" sqref="B265"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1998,2380 +2055,2534 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>96</v>
+        <v>351</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C50" t="s">
-        <v>72</v>
+        <v>352</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>92</v>
+      <c r="A51" s="1" t="s">
+        <v>353</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C51" t="s">
-        <v>92</v>
+        <v>353</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>97</v>
+        <v>354</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C52" t="s">
-        <v>74</v>
+        <v>354</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>94</v>
+      <c r="A53" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C53" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C54" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>98</v>
+      <c r="A55" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C55" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C56" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C57" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C58" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C60" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C61" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C62" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C64" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C65" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C66" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C68" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>88</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C69" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>89</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C70" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>90</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C71" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>91</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C72" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>102</v>
+      <c r="A73" t="s">
+        <v>355</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>102</v>
+        <v>356</v>
+      </c>
+      <c r="C73" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>119</v>
+      <c r="A74" t="s">
+        <v>358</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>119</v>
+        <v>357</v>
+      </c>
+      <c r="C74" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>121</v>
+      <c r="A75" t="s">
+        <v>359</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>121</v>
+        <v>359</v>
+      </c>
+      <c r="C75" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>134</v>
+        <v>360</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>134</v>
+        <v>360</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>134</v>
+        <v>360</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>135</v>
+        <v>361</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>135</v>
+        <v>361</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>135</v>
+        <v>361</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>158</v>
+        <v>362</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>158</v>
+        <v>362</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>158</v>
+        <v>362</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>159</v>
+        <v>363</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>159</v>
+        <v>364</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>159</v>
+        <v>363</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>170</v>
+        <v>366</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>160</v>
+        <v>365</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>170</v>
+        <v>366</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>97</v>
+        <v>161</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>74</v>
+        <v>161</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>94</v>
+      <c r="A131" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>94</v>
+        <v>171</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>101</v>
+        <v>163</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>101</v>
+        <v>163</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>191</v>
+        <v>164</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>338</v>
+        <v>166</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>51</v>
+        <v>167</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>51</v>
+        <v>167</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>119</v>
+        <v>169</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>119</v>
+        <v>169</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>182</v>
+        <v>367</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>196</v>
+        <v>367</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>182</v>
+        <v>367</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>172</v>
+        <v>368</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>197</v>
+        <v>368</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>172</v>
+        <v>368</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>158</v>
+        <v>369</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>198</v>
+        <v>369</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>158</v>
+        <v>369</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>133</v>
+        <v>173</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>133</v>
+        <v>173</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>56</v>
+        <v>150</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>56</v>
+        <v>150</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>218</v>
+        <v>97</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>183</v>
+        <v>74</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
-        <v>218</v>
+      <c r="A145" t="s">
+        <v>94</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>341</v>
+        <v>189</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>218</v>
+        <v>94</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>58</v>
+        <v>174</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>58</v>
+        <v>174</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>205</v>
+        <v>338</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>177</v>
+        <v>51</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>177</v>
+        <v>51</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>113</v>
+        <v>176</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>113</v>
+        <v>176</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>87</v>
+      <c r="A153" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>87</v>
+        <v>182</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>89</v>
+      <c r="A154" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>89</v>
+        <v>172</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>184</v>
+        <v>133</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>184</v>
+        <v>133</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>185</v>
+        <v>56</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>185</v>
+        <v>56</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>91</v>
+      <c r="A158" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>91</v>
+        <v>183</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>116</v>
+        <v>218</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>215</v>
+        <v>341</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>116</v>
+        <v>218</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>87</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>89</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>91</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B160" s="1" t="s">
+      <c r="B174" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C160" s="1" t="s">
+      <c r="C174" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" s="1" t="s">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B161" s="1" t="s">
+      <c r="B175" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C161" s="1" t="s">
+      <c r="C175" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B162" s="1" t="s">
+      <c r="B176" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C162" s="1" t="s">
+      <c r="C176" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B163" s="1" t="s">
+      <c r="B177" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C163" s="1" t="s">
+      <c r="C177" s="1" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E164" s="1"/>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E165" s="1"/>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="C169" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C170" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="C173" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>94</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>87</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="C175" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>89</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>91</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>133</v>
+        <v>180</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="E178" s="1"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>148</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E179" s="1"/>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>172</v>
+        <v>113</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>172</v>
+        <v>113</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>170</v>
+        <v>51</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>170</v>
+        <v>51</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>184</v>
+        <v>56</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>184</v>
+        <v>56</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>174</v>
+        <v>58</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E186" s="1"/>
+        <v>58</v>
+      </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>177</v>
+        <v>97</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>177</v>
+        <v>74</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" s="1" t="s">
-        <v>185</v>
+      <c r="A188" t="s">
+        <v>94</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>185</v>
+        <v>94</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A189" s="1" t="s">
-        <v>181</v>
+      <c r="A189" t="s">
+        <v>87</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>181</v>
+        <v>87</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" s="1" t="s">
-        <v>218</v>
+      <c r="A190" t="s">
+        <v>89</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>183</v>
+        <v>89</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" s="1" t="s">
-        <v>218</v>
+      <c r="A191" t="s">
+        <v>91</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>342</v>
+        <v>321</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>218</v>
+        <v>91</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E200" s="1"/>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B192" s="1" t="s">
+      <c r="B206" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="C192" s="1" t="s">
+      <c r="C206" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193" s="1" t="s">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B193" s="1" t="s">
+      <c r="B207" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C193" s="1" t="s">
+      <c r="C207" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="1" t="s">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B194" s="1" t="s">
+      <c r="B208" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C194" s="1" t="s">
+      <c r="C208" s="1" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C195" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C196" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>95</v>
-      </c>
-      <c r="B197" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C197" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C198" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B199" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C199" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="C200" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="C201" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C202" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A203" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C203" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C204" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A206" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C206" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="C207" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C208" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>236</v>
+        <v>179</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>250</v>
+        <v>337</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>236</v>
+        <v>179</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>159</v>
+        <v>239</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>159</v>
+        <v>239</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" s="1" t="s">
-        <v>237</v>
+      <c r="A211" t="s">
+        <v>95</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>237</v>
+        <v>95</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>55</v>
+        <v>230</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>55</v>
+        <v>230</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>118</v>
+        <v>272</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>118</v>
+        <v>231</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>222</v>
+        <v>272</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>255</v>
+        <v>347</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>222</v>
+        <v>346</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>135</v>
+        <v>233</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>135</v>
+        <v>233</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>138</v>
+        <v>221</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>260</v>
+        <v>343</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>138</v>
+        <v>221</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>161</v>
+        <v>273</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>161</v>
+        <v>234</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>238</v>
+        <v>273</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>262</v>
+        <v>344</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>226</v>
+        <v>159</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>226</v>
+        <v>159</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
-        <v>88</v>
+      <c r="A225" s="1" t="s">
+        <v>237</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>88</v>
+        <v>237</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>232</v>
+        <v>55</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>232</v>
+        <v>55</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>227</v>
+        <v>118</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>227</v>
+        <v>118</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>64</v>
+        <v>135</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>64</v>
+        <v>135</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>226</v>
+        <v>136</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>226</v>
+        <v>136</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>239</v>
+        <v>138</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>239</v>
+        <v>138</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>236</v>
+        <v>161</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>236</v>
+        <v>161</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>121</v>
+        <v>225</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>121</v>
+        <v>225</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>118</v>
+        <v>226</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>118</v>
+        <v>226</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239" s="1" t="s">
-        <v>272</v>
+      <c r="A239" t="s">
+        <v>88</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>231</v>
+        <v>88</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
-        <v>272</v>
+        <v>232</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>345</v>
+        <v>267</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>346</v>
+        <v>232</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>55</v>
+        <v>228</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>55</v>
+        <v>228</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B243" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="C243" s="1" t="s">
+      <c r="B244" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C244" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
-        <v>95</v>
-      </c>
-      <c r="B244" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="C244" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
-        <v>88</v>
+      <c r="A245" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>88</v>
+        <v>226</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>135</v>
+        <v>229</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>135</v>
+        <v>229</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>136</v>
+        <v>239</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>136</v>
+        <v>239</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>138</v>
+        <v>236</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>138</v>
+        <v>236</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>273</v>
+        <v>121</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>234</v>
+        <v>121</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
-        <v>273</v>
+        <v>118</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>348</v>
+        <v>281</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>349</v>
+        <v>118</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>159</v>
+        <v>272</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>159</v>
+        <v>231</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>161</v>
+        <v>272</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>295</v>
+        <v>345</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>161</v>
+        <v>346</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>237</v>
+        <v>55</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>237</v>
+        <v>55</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>230</v>
+        <v>64</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>230</v>
+        <v>64</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A258" s="1" t="s">
-        <v>232</v>
+      <c r="A258" t="s">
+        <v>95</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>232</v>
+        <v>95</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A259" s="1" t="s">
-        <v>222</v>
+      <c r="A259" t="s">
+        <v>88</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>222</v>
+        <v>88</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>228</v>
+        <v>135</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>228</v>
+        <v>135</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>219</v>
+        <v>136</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>219</v>
+        <v>136</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>225</v>
+        <v>138</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>225</v>
+        <v>138</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>350</v>
+        <v>292</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B265" s="1" t="s">
+      <c r="B279" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C265" s="1" t="s">
+      <c r="C279" s="1" t="s">
         <v>235</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated models to include EFL Championship
</commit_message>
<xml_diff>
--- a/Soccer Machine/Club Names.xlsx
+++ b/Soccer Machine/Club Names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\SportsStuff\TheMachine\the-machine\Soccer Machine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BCA985-0AA4-49A9-96A7-EF454C6E1CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D67E4FF-E113-432C-96E8-2C350BE86EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="3804" windowWidth="23256" windowHeight="12576" xr2:uid="{66BF1EEF-F4F0-4B2A-B933-3562F007E550}"/>
+    <workbookView xWindow="-16320" yWindow="-6615" windowWidth="16440" windowHeight="28440" xr2:uid="{66BF1EEF-F4F0-4B2A-B933-3562F007E550}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="398">
   <si>
     <t>Atlanta Utd</t>
   </si>
@@ -1147,6 +1147,90 @@
   </si>
   <si>
     <t>Monza</t>
+  </si>
+  <si>
+    <t>Bristol City</t>
+  </si>
+  <si>
+    <t>Coventry City</t>
+  </si>
+  <si>
+    <t>Hull City</t>
+  </si>
+  <si>
+    <t>Luton Town</t>
+  </si>
+  <si>
+    <t>Preston North End</t>
+  </si>
+  <si>
+    <t>West Bromwich Albion</t>
+  </si>
+  <si>
+    <t>Birmingham City</t>
+  </si>
+  <si>
+    <t>Cardiff City</t>
+  </si>
+  <si>
+    <t>Huddersfield Town</t>
+  </si>
+  <si>
+    <t>Wigan Athletic</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>Blackburn Rovers</t>
+  </si>
+  <si>
+    <t>Blackpool</t>
+  </si>
+  <si>
+    <t>Middlesbrough</t>
+  </si>
+  <si>
+    <t>Millwall</t>
+  </si>
+  <si>
+    <t>Queens Park Rangers</t>
+  </si>
+  <si>
+    <t>Rotherham United</t>
+  </si>
+  <si>
+    <t>Sheffield United</t>
+  </si>
+  <si>
+    <t>Stoke City</t>
+  </si>
+  <si>
+    <t>Sunderland</t>
+  </si>
+  <si>
+    <t>Swansea City</t>
+  </si>
+  <si>
+    <t>Huddersfield</t>
+  </si>
+  <si>
+    <t>Rotherham Utd</t>
+  </si>
+  <si>
+    <t>Blackburn</t>
+  </si>
+  <si>
+    <t>Preston</t>
+  </si>
+  <si>
+    <t>QPR</t>
+  </si>
+  <si>
+    <t>Sheffield Utd</t>
+  </si>
+  <si>
+    <t>West Brom</t>
   </si>
 </sst>
 </file>
@@ -1501,10 +1585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C69D7B6-E6BC-4B78-B3F8-3995E9E68E3A}">
-  <dimension ref="A1:E279"/>
+  <dimension ref="A1:E303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
+    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
+      <selection activeCell="A303" sqref="A303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4586,6 +4670,270 @@
         <v>235</v>
       </c>
     </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>370</v>
+      </c>
+      <c r="B280" t="s">
+        <v>370</v>
+      </c>
+      <c r="C280" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>371</v>
+      </c>
+      <c r="B281" t="s">
+        <v>371</v>
+      </c>
+      <c r="C281" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>372</v>
+      </c>
+      <c r="B282" t="s">
+        <v>372</v>
+      </c>
+      <c r="C282" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>373</v>
+      </c>
+      <c r="B283" t="s">
+        <v>373</v>
+      </c>
+      <c r="C283" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>374</v>
+      </c>
+      <c r="B284" t="s">
+        <v>394</v>
+      </c>
+      <c r="C284" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>375</v>
+      </c>
+      <c r="B285" t="s">
+        <v>397</v>
+      </c>
+      <c r="C285" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>376</v>
+      </c>
+      <c r="B286" t="s">
+        <v>376</v>
+      </c>
+      <c r="C286" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>50</v>
+      </c>
+      <c r="B287" t="s">
+        <v>50</v>
+      </c>
+      <c r="C287" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>377</v>
+      </c>
+      <c r="B288" t="s">
+        <v>377</v>
+      </c>
+      <c r="C288" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>378</v>
+      </c>
+      <c r="B289" t="s">
+        <v>391</v>
+      </c>
+      <c r="C289" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>60</v>
+      </c>
+      <c r="B290" t="s">
+        <v>60</v>
+      </c>
+      <c r="C290" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>379</v>
+      </c>
+      <c r="B291" t="s">
+        <v>379</v>
+      </c>
+      <c r="C291" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>380</v>
+      </c>
+      <c r="B292" t="s">
+        <v>380</v>
+      </c>
+      <c r="C292" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>381</v>
+      </c>
+      <c r="B293" t="s">
+        <v>393</v>
+      </c>
+      <c r="C293" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>382</v>
+      </c>
+      <c r="B294" t="s">
+        <v>382</v>
+      </c>
+      <c r="C294" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>383</v>
+      </c>
+      <c r="B295" t="s">
+        <v>383</v>
+      </c>
+      <c r="C295" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>384</v>
+      </c>
+      <c r="B296" t="s">
+        <v>384</v>
+      </c>
+      <c r="C296" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>385</v>
+      </c>
+      <c r="B297" t="s">
+        <v>395</v>
+      </c>
+      <c r="C297" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>386</v>
+      </c>
+      <c r="B298" t="s">
+        <v>392</v>
+      </c>
+      <c r="C298" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>387</v>
+      </c>
+      <c r="B299" t="s">
+        <v>396</v>
+      </c>
+      <c r="C299" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>388</v>
+      </c>
+      <c r="B300" t="s">
+        <v>388</v>
+      </c>
+      <c r="C300" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>389</v>
+      </c>
+      <c r="B301" t="s">
+        <v>389</v>
+      </c>
+      <c r="C301" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>390</v>
+      </c>
+      <c r="B302" t="s">
+        <v>390</v>
+      </c>
+      <c r="C302" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>63</v>
+      </c>
+      <c r="B303" t="s">
+        <v>63</v>
+      </c>
+      <c r="C303" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Liga MX to daily picks
</commit_message>
<xml_diff>
--- a/Soccer Machine/Club Names.xlsx
+++ b/Soccer Machine/Club Names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\SportsStuff\TheMachine\the-machine\Soccer Machine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D67E4FF-E113-432C-96E8-2C350BE86EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE65AAB2-39C5-4789-A80D-C22424C2EAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-6615" windowWidth="16440" windowHeight="28440" xr2:uid="{66BF1EEF-F4F0-4B2A-B933-3562F007E550}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="431">
   <si>
     <t>Atlanta Utd</t>
   </si>
@@ -1231,6 +1231,105 @@
   </si>
   <si>
     <t>West Brom</t>
+  </si>
+  <si>
+    <t>América</t>
+  </si>
+  <si>
+    <t>Atlas</t>
+  </si>
+  <si>
+    <t>Atlético</t>
+  </si>
+  <si>
+    <t>Cruz Azul</t>
+  </si>
+  <si>
+    <t>FC Juárez</t>
+  </si>
+  <si>
+    <t>Guadalajara</t>
+  </si>
+  <si>
+    <t>León</t>
+  </si>
+  <si>
+    <t>Mazatlán</t>
+  </si>
+  <si>
+    <t>Monterrey</t>
+  </si>
+  <si>
+    <t>Necaxa</t>
+  </si>
+  <si>
+    <t>Pachuca</t>
+  </si>
+  <si>
+    <t>Puebla</t>
+  </si>
+  <si>
+    <t>Querétaro</t>
+  </si>
+  <si>
+    <t>Santos</t>
+  </si>
+  <si>
+    <t>Tijuana</t>
+  </si>
+  <si>
+    <t>Toluca</t>
+  </si>
+  <si>
+    <t>UANL</t>
+  </si>
+  <si>
+    <t>UNAM</t>
+  </si>
+  <si>
+    <t>Atlas FC</t>
+  </si>
+  <si>
+    <t>Atletico San Luis</t>
+  </si>
+  <si>
+    <t>CF Monterrey</t>
+  </si>
+  <si>
+    <t>CF Pachuca</t>
+  </si>
+  <si>
+    <t>Chivas Guadalajara</t>
+  </si>
+  <si>
+    <t>Club America</t>
+  </si>
+  <si>
+    <t>Club Leon</t>
+  </si>
+  <si>
+    <t>Deportivo Toluca FC</t>
+  </si>
+  <si>
+    <t>FC Juarez</t>
+  </si>
+  <si>
+    <t>Mazatlan FC</t>
+  </si>
+  <si>
+    <t>Puebla FC</t>
+  </si>
+  <si>
+    <t>Pumas UNAM</t>
+  </si>
+  <si>
+    <t>Queretaro FC</t>
+  </si>
+  <si>
+    <t>Santos Laguna</t>
+  </si>
+  <si>
+    <t>Tigres UANL</t>
   </si>
 </sst>
 </file>
@@ -1585,10 +1684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C69D7B6-E6BC-4B78-B3F8-3995E9E68E3A}">
-  <dimension ref="A1:E303"/>
+  <dimension ref="A1:E321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
-      <selection activeCell="A303" sqref="A303"/>
+    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
+      <selection activeCell="E304" sqref="E304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4934,6 +5033,204 @@
         <v>63</v>
       </c>
     </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>421</v>
+      </c>
+      <c r="B304" t="s">
+        <v>398</v>
+      </c>
+      <c r="C304" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>416</v>
+      </c>
+      <c r="B305" t="s">
+        <v>399</v>
+      </c>
+      <c r="C305" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>417</v>
+      </c>
+      <c r="B306" t="s">
+        <v>400</v>
+      </c>
+      <c r="C306" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>401</v>
+      </c>
+      <c r="B307" t="s">
+        <v>401</v>
+      </c>
+      <c r="C307" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>424</v>
+      </c>
+      <c r="B308" t="s">
+        <v>402</v>
+      </c>
+      <c r="C308" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>420</v>
+      </c>
+      <c r="B309" t="s">
+        <v>403</v>
+      </c>
+      <c r="C309" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>422</v>
+      </c>
+      <c r="B310" t="s">
+        <v>404</v>
+      </c>
+      <c r="C310" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>425</v>
+      </c>
+      <c r="B311" t="s">
+        <v>405</v>
+      </c>
+      <c r="C311" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>418</v>
+      </c>
+      <c r="B312" t="s">
+        <v>406</v>
+      </c>
+      <c r="C312" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>407</v>
+      </c>
+      <c r="B313" t="s">
+        <v>407</v>
+      </c>
+      <c r="C313" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>419</v>
+      </c>
+      <c r="B314" t="s">
+        <v>408</v>
+      </c>
+      <c r="C314" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>426</v>
+      </c>
+      <c r="B315" t="s">
+        <v>409</v>
+      </c>
+      <c r="C315" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>428</v>
+      </c>
+      <c r="B316" t="s">
+        <v>410</v>
+      </c>
+      <c r="C316" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>429</v>
+      </c>
+      <c r="B317" t="s">
+        <v>411</v>
+      </c>
+      <c r="C317" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>412</v>
+      </c>
+      <c r="B318" t="s">
+        <v>412</v>
+      </c>
+      <c r="C318" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>423</v>
+      </c>
+      <c r="B319" t="s">
+        <v>413</v>
+      </c>
+      <c r="C319" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>430</v>
+      </c>
+      <c r="B320" t="s">
+        <v>414</v>
+      </c>
+      <c r="C320" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>427</v>
+      </c>
+      <c r="B321" t="s">
+        <v>415</v>
+      </c>
+      <c r="C321" t="s">
+        <v>427</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update club names file
</commit_message>
<xml_diff>
--- a/Soccer Machine/Club Names.xlsx
+++ b/Soccer Machine/Club Names.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\SportsStuff\TheMachine\the-machine\Soccer Machine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71920B70-586B-481F-BA86-879606434EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259FAF8D-BF45-4267-B785-85A922EB6152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-10095" windowWidth="16440" windowHeight="28440" xr2:uid="{66BF1EEF-F4F0-4B2A-B933-3562F007E550}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="469">
   <si>
     <t>Atlanta Utd</t>
   </si>
@@ -1414,6 +1414,36 @@
   </si>
   <si>
     <t>Botafogo</t>
+  </si>
+  <si>
+    <t>Las Palmas</t>
+  </si>
+  <si>
+    <t>Darmstadt 98</t>
+  </si>
+  <si>
+    <t>Darmstadt</t>
+  </si>
+  <si>
+    <t>Heidenheim</t>
+  </si>
+  <si>
+    <t>Le Havre</t>
+  </si>
+  <si>
+    <t>Frosinone</t>
+  </si>
+  <si>
+    <t>Sheffield Weds</t>
+  </si>
+  <si>
+    <t>Sheffield Wednesday</t>
+  </si>
+  <si>
+    <t>Plymouth Argyle</t>
+  </si>
+  <si>
+    <t>Ipswich Town</t>
   </si>
 </sst>
 </file>
@@ -1768,10 +1798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C69D7B6-E6BC-4B78-B3F8-3995E9E68E3A}">
-  <dimension ref="A1:E341"/>
+  <dimension ref="A1:E349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="D330" sqref="D330"/>
+    <sheetView tabSelected="1" topLeftCell="A314" workbookViewId="0">
+      <selection activeCell="C279" sqref="C279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2607,2931 +2637,3019 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>117</v>
+      <c r="A76" t="s">
+        <v>459</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>117</v>
+        <v>459</v>
+      </c>
+      <c r="C76" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>360</v>
+        <v>116</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>360</v>
+        <v>116</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>360</v>
+        <v>116</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>128</v>
+        <v>361</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>128</v>
+        <v>361</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>128</v>
+        <v>361</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>129</v>
+        <v>461</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>129</v>
+        <v>460</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>129</v>
+        <v>461</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>130</v>
+        <v>462</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>130</v>
+        <v>462</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>130</v>
+        <v>462</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>362</v>
+        <v>149</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>362</v>
+        <v>145</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>362</v>
+        <v>145</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>363</v>
+        <v>146</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>364</v>
+        <v>146</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>363</v>
+        <v>146</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>366</v>
+        <v>147</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>365</v>
+        <v>147</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>366</v>
+        <v>147</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>150</v>
+        <v>362</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>150</v>
+        <v>362</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>150</v>
+        <v>362</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>151</v>
+        <v>363</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>151</v>
+        <v>364</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>151</v>
+        <v>363</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>152</v>
+        <v>366</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>152</v>
+        <v>365</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>152</v>
+        <v>366</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>153</v>
+        <v>463</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>153</v>
+        <v>463</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>153</v>
+        <v>463</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>367</v>
+        <v>166</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>367</v>
+        <v>166</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>367</v>
+        <v>166</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>368</v>
+        <v>167</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>368</v>
+        <v>167</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>368</v>
+        <v>167</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>369</v>
+        <v>168</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>369</v>
+        <v>168</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>369</v>
+        <v>168</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>150</v>
+        <v>367</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>187</v>
+        <v>367</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>150</v>
+        <v>367</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>97</v>
+        <v>368</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>188</v>
+        <v>368</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>74</v>
+        <v>368</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>94</v>
+      <c r="A145" s="1" t="s">
+        <v>369</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>189</v>
+        <v>369</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>94</v>
+        <v>369</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>101</v>
+        <v>464</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>190</v>
+        <v>464</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>101</v>
+        <v>464</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>175</v>
+        <v>97</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>338</v>
+        <v>188</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>175</v>
+        <v>74</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
-        <v>51</v>
+      <c r="A150" t="s">
+        <v>94</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>176</v>
+        <v>101</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>176</v>
+        <v>101</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>119</v>
+        <v>174</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>119</v>
+        <v>174</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>197</v>
+        <v>338</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>158</v>
+        <v>51</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>158</v>
+        <v>51</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>133</v>
+        <v>176</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>133</v>
+        <v>176</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>218</v>
+        <v>172</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>341</v>
+        <v>197</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>218</v>
+        <v>172</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>57</v>
+        <v>158</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>57</v>
+        <v>158</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>58</v>
+        <v>133</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>58</v>
+        <v>133</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>170</v>
+        <v>56</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>170</v>
+        <v>56</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>148</v>
+        <v>218</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>177</v>
+        <v>218</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>206</v>
+        <v>341</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>177</v>
+        <v>218</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>178</v>
+        <v>58</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>178</v>
+        <v>58</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>87</v>
+      <c r="A167" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>87</v>
+        <v>170</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>89</v>
+      <c r="A168" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>89</v>
+        <v>148</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>184</v>
+        <v>113</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>184</v>
+        <v>113</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" s="1" t="s">
-        <v>116</v>
+      <c r="A173" t="s">
+        <v>89</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>306</v>
+        <v>213</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" s="1" t="s">
-        <v>176</v>
+      <c r="A177" t="s">
+        <v>91</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>307</v>
+        <v>214</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>176</v>
+        <v>91</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>180</v>
+        <v>116</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>308</v>
+        <v>215</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>180</v>
+        <v>116</v>
       </c>
       <c r="E178" s="1"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>101</v>
+        <v>180</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>309</v>
+        <v>216</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>101</v>
+        <v>180</v>
       </c>
       <c r="E179" s="1"/>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>119</v>
+        <v>181</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>310</v>
+        <v>217</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>119</v>
+        <v>181</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>113</v>
+        <v>178</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>113</v>
+        <v>178</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>116</v>
+        <v>176</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>116</v>
+        <v>176</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>51</v>
+        <v>180</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>51</v>
+        <v>180</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>94</v>
+      <c r="A188" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>87</v>
+      <c r="A189" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>89</v>
+      <c r="A190" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>91</v>
+      <c r="A191" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>133</v>
+        <v>74</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A193" s="1" t="s">
-        <v>148</v>
+      <c r="A193" t="s">
+        <v>94</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A194" s="1" t="s">
-        <v>150</v>
+      <c r="A194" t="s">
+        <v>87</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>150</v>
+        <v>87</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A195" s="1" t="s">
-        <v>172</v>
+      <c r="A195" t="s">
+        <v>89</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>172</v>
+        <v>89</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A196" s="1" t="s">
-        <v>158</v>
+      <c r="A196" t="s">
+        <v>91</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>170</v>
+        <v>133</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>170</v>
+        <v>133</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E200" s="1"/>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>218</v>
+        <v>174</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>218</v>
+        <v>174</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>179</v>
+        <v>218</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>240</v>
+        <v>342</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>95</v>
+      <c r="A211" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>241</v>
+        <v>335</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>95</v>
+        <v>175</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>230</v>
+        <v>175</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>242</v>
+        <v>339</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>230</v>
+        <v>175</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>272</v>
+        <v>182</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>243</v>
+        <v>336</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>231</v>
+        <v>182</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>272</v>
+        <v>179</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>346</v>
+        <v>179</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216" s="1" t="s">
-        <v>233</v>
+      <c r="A216" t="s">
+        <v>95</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>233</v>
+        <v>95</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>121</v>
+        <v>230</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>121</v>
+        <v>230</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>221</v>
+        <v>272</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>221</v>
+        <v>272</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>221</v>
+        <v>346</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>273</v>
+        <v>219</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>273</v>
+        <v>233</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>344</v>
+        <v>245</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>235</v>
+        <v>121</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>235</v>
+        <v>121</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>159</v>
+        <v>221</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>251</v>
+        <v>343</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>159</v>
+        <v>221</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>237</v>
+        <v>273</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>55</v>
+        <v>273</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>253</v>
+        <v>344</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>55</v>
+        <v>234</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>118</v>
+        <v>235</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>118</v>
+        <v>235</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>223</v>
+        <v>159</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>223</v>
+        <v>159</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>135</v>
+        <v>237</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>135</v>
+        <v>237</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>136</v>
+        <v>55</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>136</v>
+        <v>55</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>220</v>
+        <v>118</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>220</v>
+        <v>118</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>161</v>
+        <v>223</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>161</v>
+        <v>223</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>238</v>
+        <v>135</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>238</v>
+        <v>135</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>224</v>
+        <v>136</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>224</v>
+        <v>136</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>226</v>
+        <v>138</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>226</v>
+        <v>138</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
-        <v>88</v>
+      <c r="A239" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>88</v>
+        <v>161</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244" s="1" t="s">
-        <v>64</v>
+      <c r="A244" t="s">
+        <v>88</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>223</v>
+        <v>64</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>223</v>
+        <v>64</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>121</v>
+        <v>229</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>121</v>
+        <v>229</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
-        <v>118</v>
+        <v>239</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>118</v>
+        <v>239</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>272</v>
+        <v>236</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>272</v>
+        <v>223</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>345</v>
+        <v>278</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>346</v>
+        <v>223</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>55</v>
+        <v>121</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>55</v>
+        <v>121</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A258" t="s">
-        <v>95</v>
+      <c r="A258" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>95</v>
+        <v>231</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A259" t="s">
-        <v>88</v>
+      <c r="A259" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>287</v>
+        <v>345</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>88</v>
+        <v>346</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>135</v>
+        <v>220</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>135</v>
+        <v>220</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>136</v>
+        <v>55</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>136</v>
+        <v>55</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>138</v>
+        <v>64</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>138</v>
+        <v>64</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A263" s="1" t="s">
-        <v>238</v>
+      <c r="A263" t="s">
+        <v>95</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>238</v>
+        <v>95</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A264" s="1" t="s">
-        <v>233</v>
+      <c r="A264" t="s">
+        <v>88</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>233</v>
+        <v>88</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>273</v>
+        <v>135</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>234</v>
+        <v>135</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>273</v>
+        <v>136</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>348</v>
+        <v>289</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>349</v>
+        <v>136</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>161</v>
+        <v>238</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>161</v>
+        <v>238</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>237</v>
+        <v>273</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>230</v>
+        <v>273</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>298</v>
+        <v>348</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>230</v>
+        <v>349</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>232</v>
+        <v>159</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>232</v>
+        <v>159</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>222</v>
+        <v>161</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>222</v>
+        <v>161</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>219</v>
+        <v>237</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>219</v>
+        <v>237</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B279" s="1" t="s">
+      <c r="B284" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C279" s="1" t="s">
+      <c r="C284" s="1" t="s">
         <v>235</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
-        <v>370</v>
-      </c>
-      <c r="B280" t="s">
-        <v>370</v>
-      </c>
-      <c r="C280" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A281" t="s">
-        <v>371</v>
-      </c>
-      <c r="B281" t="s">
-        <v>371</v>
-      </c>
-      <c r="C281" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A282" t="s">
-        <v>372</v>
-      </c>
-      <c r="B282" t="s">
-        <v>372</v>
-      </c>
-      <c r="C282" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A283" t="s">
-        <v>373</v>
-      </c>
-      <c r="B283" t="s">
-        <v>373</v>
-      </c>
-      <c r="C283" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A284" t="s">
-        <v>374</v>
-      </c>
-      <c r="B284" t="s">
-        <v>394</v>
-      </c>
-      <c r="C284" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B285" t="s">
-        <v>397</v>
+        <v>370</v>
       </c>
       <c r="C285" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B286" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C286" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>50</v>
+        <v>372</v>
       </c>
       <c r="B287" t="s">
-        <v>50</v>
+        <v>372</v>
       </c>
       <c r="C287" t="s">
-        <v>50</v>
+        <v>372</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B288" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C288" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B289" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="C289" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>60</v>
+        <v>375</v>
       </c>
       <c r="B290" t="s">
-        <v>60</v>
+        <v>397</v>
       </c>
       <c r="C290" t="s">
-        <v>60</v>
+        <v>375</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B291" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C291" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>380</v>
+        <v>50</v>
       </c>
       <c r="B292" t="s">
-        <v>380</v>
+        <v>50</v>
       </c>
       <c r="C292" t="s">
-        <v>380</v>
+        <v>50</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B293" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="C293" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B294" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="C294" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>383</v>
+        <v>60</v>
       </c>
       <c r="B295" t="s">
-        <v>383</v>
+        <v>60</v>
       </c>
       <c r="C295" t="s">
-        <v>383</v>
+        <v>60</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="B296" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C296" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B297" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="C297" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B298" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C298" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B299" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="C299" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="B300" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C300" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B301" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C301" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="B302" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="C302" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>63</v>
+        <v>386</v>
       </c>
       <c r="B303" t="s">
-        <v>63</v>
+        <v>392</v>
       </c>
       <c r="C303" t="s">
-        <v>63</v>
+        <v>386</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>421</v>
+        <v>387</v>
       </c>
       <c r="B304" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C304" t="s">
-        <v>421</v>
+        <v>387</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>416</v>
+        <v>388</v>
       </c>
       <c r="B305" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="C305" t="s">
-        <v>416</v>
+        <v>388</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>417</v>
+        <v>389</v>
       </c>
       <c r="B306" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
       <c r="C306" t="s">
-        <v>417</v>
+        <v>389</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="B307" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="C307" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>424</v>
+        <v>63</v>
       </c>
       <c r="B308" t="s">
-        <v>402</v>
+        <v>63</v>
       </c>
       <c r="C308" t="s">
-        <v>424</v>
+        <v>63</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>420</v>
+        <v>466</v>
       </c>
       <c r="B309" t="s">
-        <v>403</v>
+        <v>465</v>
       </c>
       <c r="C309" t="s">
-        <v>420</v>
+        <v>466</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>422</v>
+        <v>467</v>
       </c>
       <c r="B310" t="s">
-        <v>404</v>
+        <v>467</v>
       </c>
       <c r="C310" t="s">
-        <v>422</v>
+        <v>467</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>425</v>
+        <v>468</v>
       </c>
       <c r="B311" t="s">
-        <v>405</v>
+        <v>468</v>
       </c>
       <c r="C311" t="s">
-        <v>425</v>
+        <v>468</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B312" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="C312" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
       <c r="B313" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="C313" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B314" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="C314" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>426</v>
+        <v>401</v>
       </c>
       <c r="B315" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="C315" t="s">
-        <v>426</v>
+        <v>401</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B316" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="C316" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="B317" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C317" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
       <c r="B318" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="C318" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B319" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="C319" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="B320" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="C320" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
+        <v>407</v>
+      </c>
+      <c r="B321" t="s">
+        <v>407</v>
+      </c>
+      <c r="C321" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>419</v>
+      </c>
+      <c r="B322" t="s">
+        <v>408</v>
+      </c>
+      <c r="C322" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>426</v>
+      </c>
+      <c r="B323" t="s">
+        <v>409</v>
+      </c>
+      <c r="C323" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>428</v>
+      </c>
+      <c r="B324" t="s">
+        <v>410</v>
+      </c>
+      <c r="C324" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>429</v>
+      </c>
+      <c r="B325" t="s">
+        <v>411</v>
+      </c>
+      <c r="C325" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>412</v>
+      </c>
+      <c r="B326" t="s">
+        <v>412</v>
+      </c>
+      <c r="C326" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>423</v>
+      </c>
+      <c r="B327" t="s">
+        <v>413</v>
+      </c>
+      <c r="C327" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>430</v>
+      </c>
+      <c r="B328" t="s">
+        <v>414</v>
+      </c>
+      <c r="C328" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
         <v>427</v>
       </c>
-      <c r="B321" t="s">
+      <c r="B329" t="s">
         <v>415</v>
       </c>
-      <c r="C321" t="s">
+      <c r="C329" t="s">
         <v>427</v>
-      </c>
-    </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A322" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="B322" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="C322" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A323" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="B323" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="C323" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A324" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="B324" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="C324" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A325" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="B325" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C325" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A326" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="B326" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="C326" s="1" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A327" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="B327" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C327" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A328" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="B328" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="C328" s="1" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A329" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="B329" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="C329" s="1" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="C330" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
-        <v>454</v>
+        <v>435</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="C336" s="1" t="s">
-        <v>454</v>
+        <v>435</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
-        <v>411</v>
+        <v>438</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>411</v>
+        <v>438</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>411</v>
+        <v>438</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A342" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A343" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A344" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A345" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B345" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A346" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A347" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A348" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A349" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="B341" s="1" t="s">
+      <c r="B349" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="C341" s="1" t="s">
+      <c r="C349" s="1" t="s">
         <v>443</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated models for 2023-2024
</commit_message>
<xml_diff>
--- a/Soccer Machine/Club Names.xlsx
+++ b/Soccer Machine/Club Names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\SportsStuff\TheMachine\the-machine\Soccer Machine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B63548-DD82-4F90-898C-24120EA39F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527DEE45-EE64-4091-84C2-22F8A912D92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-10095" windowWidth="16440" windowHeight="28440" xr2:uid="{66BF1EEF-F4F0-4B2A-B933-3562F007E550}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="305">
   <si>
     <t>Atlanta Utd</t>
   </si>
@@ -949,6 +949,9 @@
   </si>
   <si>
     <t>Union SG</t>
+  </si>
+  <si>
+    <t>Atletico Mineiro</t>
   </si>
 </sst>
 </file>
@@ -1313,7 +1316,7 @@
   <dimension ref="A1:E220"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="B212" sqref="B212"/>
+      <selection activeCell="B192" sqref="B192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3450,13 +3453,13 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>275</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>